<commit_message>
added more contacts in statisitc
</commit_message>
<xml_diff>
--- a/output/test_results_03122022.xlsx
+++ b/output/test_results_03122022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="26">
   <si>
     <t>Case Number</t>
   </si>
@@ -90,12 +90,15 @@
   <si>
     <t>Missed Handwash</t>
   </si>
+  <si>
+    <t>missed contacts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,6 +117,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,10 +269,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -292,6 +312,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -600,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -622,59 +645,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="19" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="13" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="16" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="16" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="14"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="17"/>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
@@ -699,7 +722,7 @@
       <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="14"/>
+      <c r="L3" s="17"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1036,7 +1059,7 @@
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="23">
         <v>1</v>
       </c>
       <c r="I12" s="3">
@@ -1048,7 +1071,7 @@
       <c r="K12" s="4">
         <v>0</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="M12" s="5"/>
@@ -1231,7 +1254,7 @@
       <c r="G17" s="2">
         <v>1</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="23">
         <v>0</v>
       </c>
       <c r="I17" s="3">
@@ -1243,7 +1266,7 @@
       <c r="K17" s="4">
         <v>0</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="8" t="s">
         <v>20</v>
       </c>
       <c r="M17" s="5"/>
@@ -1312,7 +1335,7 @@
       <c r="H19" s="3">
         <v>0</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="23">
         <v>1</v>
       </c>
       <c r="J19" s="3">
@@ -1321,7 +1344,7 @@
       <c r="K19" s="4">
         <v>0</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="L19" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M19" s="5"/>
@@ -1351,7 +1374,7 @@
       <c r="H20" s="3">
         <v>1</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="23">
         <v>1</v>
       </c>
       <c r="J20" s="3">
@@ -1360,264 +1383,834 @@
       <c r="K20" s="4">
         <v>0</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="L20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="7"/>
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="11">
+        <v>1</v>
+      </c>
+      <c r="I21" s="11">
+        <v>0</v>
+      </c>
+      <c r="J21" s="11">
+        <v>1</v>
+      </c>
+      <c r="K21" s="12">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="7"/>
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>1</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0</v>
+      </c>
+      <c r="J22" s="11">
+        <v>1</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="7"/>
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+      <c r="H23" s="11">
+        <v>1</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
+        <v>1</v>
+      </c>
+      <c r="K23" s="12">
+        <v>0</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="7"/>
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11">
+        <v>1</v>
+      </c>
+      <c r="I24" s="11">
+        <v>0</v>
+      </c>
+      <c r="J24" s="11">
+        <v>1</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="7"/>
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0</v>
+      </c>
+      <c r="H25" s="11">
+        <v>1</v>
+      </c>
+      <c r="I25" s="11">
+        <v>0</v>
+      </c>
+      <c r="J25" s="11">
+        <v>1</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="7"/>
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="7"/>
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <v>0</v>
+      </c>
+      <c r="I27" s="11">
+        <v>1</v>
+      </c>
+      <c r="J27" s="11">
+        <v>1</v>
+      </c>
+      <c r="K27" s="12">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="7"/>
+      <c r="A28" s="1">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0</v>
+      </c>
+      <c r="I28" s="11">
+        <v>1</v>
+      </c>
+      <c r="J28" s="11">
+        <v>1</v>
+      </c>
+      <c r="K28" s="12">
+        <v>0</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="7"/>
+      <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10">
+        <v>1</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11">
+        <v>1</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1</v>
+      </c>
+      <c r="K29" s="12">
+        <v>0</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="7"/>
+      <c r="A30" s="1">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
+      <c r="F30" s="10">
+        <v>1</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11">
+        <v>0</v>
+      </c>
+      <c r="I30" s="11">
+        <v>1</v>
+      </c>
+      <c r="J30" s="11">
+        <v>1</v>
+      </c>
+      <c r="K30" s="12">
+        <v>0</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M30" s="5"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="7"/>
+      <c r="A31" s="1">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="10">
+        <v>1</v>
+      </c>
+      <c r="E31" s="10">
+        <v>1</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="M31" s="5"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="7"/>
+      <c r="A32" s="1">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10">
+        <v>1</v>
+      </c>
+      <c r="H32" s="11">
+        <v>1</v>
+      </c>
+      <c r="I32" s="11">
+        <v>1</v>
+      </c>
+      <c r="J32" s="11">
+        <v>0</v>
+      </c>
+      <c r="K32" s="12">
+        <v>1</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="7"/>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
+      <c r="E33" s="10">
+        <v>1</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10">
+        <v>1</v>
+      </c>
+      <c r="H33" s="11">
+        <v>1</v>
+      </c>
+      <c r="I33" s="11">
+        <v>1</v>
+      </c>
+      <c r="J33" s="11">
+        <v>0</v>
+      </c>
+      <c r="K33" s="12">
+        <v>1</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M33" s="5"/>
     </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="7"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10">
+        <v>0</v>
+      </c>
+      <c r="G34" s="10">
+        <v>1</v>
+      </c>
+      <c r="H34" s="11">
+        <v>1</v>
+      </c>
+      <c r="I34" s="11">
+        <v>1</v>
+      </c>
+      <c r="J34" s="11">
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
+        <v>1</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="7"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1</v>
+      </c>
+      <c r="H35" s="11">
+        <v>1</v>
+      </c>
+      <c r="I35" s="11">
+        <v>1</v>
+      </c>
+      <c r="J35" s="11">
+        <v>0</v>
+      </c>
+      <c r="K35" s="12">
+        <v>1</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="7"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10">
+        <v>1</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1</v>
+      </c>
+      <c r="G36" s="10">
+        <v>0</v>
+      </c>
+      <c r="H36" s="23">
+        <v>0</v>
+      </c>
+      <c r="I36" s="23">
+        <v>0</v>
+      </c>
+      <c r="J36" s="11">
+        <v>1</v>
+      </c>
+      <c r="K36" s="12">
+        <v>0</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="7"/>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10">
+        <v>1</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3">
+        <v>1</v>
+      </c>
+      <c r="K37" s="4">
+        <v>0</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="7"/>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1</v>
+      </c>
+      <c r="F38" s="10">
+        <v>1</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0</v>
+      </c>
+      <c r="H38" s="23">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1</v>
+      </c>
+      <c r="J38" s="3">
+        <v>1</v>
+      </c>
+      <c r="K38" s="4">
+        <v>0</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="M38" s="5"/>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="7"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10">
+        <v>1</v>
+      </c>
+      <c r="F39" s="10">
+        <v>1</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0</v>
+      </c>
+      <c r="H39" s="11">
+        <v>1</v>
+      </c>
+      <c r="I39" s="11">
+        <v>1</v>
+      </c>
+      <c r="J39" s="11">
+        <v>1</v>
+      </c>
+      <c r="K39" s="12">
+        <v>0</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="7"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="10">
+        <v>1</v>
+      </c>
+      <c r="E40" s="10">
+        <v>1</v>
+      </c>
+      <c r="F40" s="10">
+        <v>1</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0</v>
+      </c>
+      <c r="H40" s="11">
+        <v>1</v>
+      </c>
+      <c r="I40" s="11">
+        <v>1</v>
+      </c>
+      <c r="J40" s="11">
+        <v>1</v>
+      </c>
+      <c r="K40" s="12">
+        <v>0</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M40" s="5"/>
     </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="7"/>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="10">
+        <v>1</v>
+      </c>
+      <c r="E41" s="10">
+        <v>1</v>
+      </c>
+      <c r="F41" s="10">
+        <v>1</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0</v>
+      </c>
+      <c r="H41" s="11">
+        <v>1</v>
+      </c>
+      <c r="I41" s="11">
+        <v>1</v>
+      </c>
+      <c r="J41" s="11">
+        <v>1</v>
+      </c>
+      <c r="K41" s="12">
+        <v>0</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="M41" s="5"/>
     </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>39</v>
+      </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1629,7 +2222,10 @@
       <c r="L42" s="7"/>
       <c r="M42" s="5"/>
     </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>40</v>
+      </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -1641,7 +2237,10 @@
       <c r="L43" s="7"/>
       <c r="M43" s="5"/>
     </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>41</v>
+      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -1653,7 +2252,10 @@
       <c r="L44" s="7"/>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>42</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -1665,7 +2267,10 @@
       <c r="L45" s="7"/>
       <c r="M45" s="5"/>
     </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>43</v>
+      </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -1677,7 +2282,10 @@
       <c r="L46" s="7"/>
       <c r="M46" s="5"/>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>44</v>
+      </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -1689,7 +2297,10 @@
       <c r="L47" s="7"/>
       <c r="M47" s="5"/>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>45</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -1701,7 +2312,10 @@
       <c r="L48" s="7"/>
       <c r="M48" s="5"/>
     </row>
-    <row r="49" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>46</v>
+      </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -1713,7 +2327,10 @@
       <c r="L49" s="7"/>
       <c r="M49" s="5"/>
     </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>47</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -1725,7 +2342,10 @@
       <c r="L50" s="7"/>
       <c r="M50" s="5"/>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>48</v>
+      </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -1737,7 +2357,10 @@
       <c r="L51" s="7"/>
       <c r="M51" s="5"/>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>49</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -1749,7 +2372,10 @@
       <c r="L52" s="7"/>
       <c r="M52" s="5"/>
     </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>50</v>
+      </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -1761,7 +2387,10 @@
       <c r="L53" s="7"/>
       <c r="M53" s="5"/>
     </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>51</v>
+      </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -1773,7 +2402,10 @@
       <c r="L54" s="7"/>
       <c r="M54" s="5"/>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>52</v>
+      </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -1785,7 +2417,10 @@
       <c r="L55" s="7"/>
       <c r="M55" s="5"/>
     </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>53</v>
+      </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -1797,7 +2432,7 @@
       <c r="L56" s="7"/>
       <c r="M56" s="5"/>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -1809,7 +2444,7 @@
       <c r="L57" s="7"/>
       <c r="M57" s="5"/>
     </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -1821,7 +2456,7 @@
       <c r="L58" s="7"/>
       <c r="M58" s="5"/>
     </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -1833,7 +2468,7 @@
       <c r="L59" s="7"/>
       <c r="M59" s="5"/>
     </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -1845,7 +2480,7 @@
       <c r="L60" s="7"/>
       <c r="M60" s="5"/>
     </row>
-    <row r="61" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L61" s="6"/>
     </row>
   </sheetData>

</xml_diff>